<commit_message>
Implementacion punteros simples y con dos tipos de nodos
</commit_message>
<xml_diff>
--- a/TDA Matriz Dispersa.xlsx
+++ b/TDA Matriz Dispersa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vectores" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>toStr()=</t>
   </si>
@@ -75,12 +75,6 @@
     <t>dc =</t>
   </si>
   <si>
-    <t>aux</t>
-  </si>
-  <si>
-    <t>(2,2,10)</t>
-  </si>
-  <si>
     <t>ptrInicio</t>
   </si>
   <si>
@@ -105,18 +99,6 @@
     <t>(1,3,80)</t>
   </si>
   <si>
-    <t>rep = 0</t>
-  </si>
-  <si>
-    <t>rep = 1</t>
-  </si>
-  <si>
-    <t>nt = 3</t>
-  </si>
-  <si>
-    <t>elemento(1,3) = 0</t>
-  </si>
-  <si>
     <t>max = 25</t>
   </si>
   <si>
@@ -172,13 +154,139 @@
   </si>
   <si>
     <t>3x5</t>
+  </si>
+  <si>
+    <t>def_valor_repetido(1)</t>
+  </si>
+  <si>
+    <t>def_valor_repetido(99)</t>
+  </si>
+  <si>
+    <t>Fil</t>
+  </si>
+  <si>
+    <t>Col</t>
+  </si>
+  <si>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>sig</t>
+  </si>
+  <si>
+    <t>Nodo</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>ptrMat = A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>nuevoRepe = 1</t>
+  </si>
+  <si>
+    <t>antRepe = 0</t>
+  </si>
+  <si>
+    <t>repe = valor</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Quedan</t>
+  </si>
+  <si>
+    <t>Elim</t>
+  </si>
+  <si>
+    <t>Nuevo</t>
+  </si>
+  <si>
+    <t>nt = 11</t>
+  </si>
+  <si>
+    <t>nt = 16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,34 +330,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -279,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,26 +537,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,9 +547,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,7 +809,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>f = 2</a:t>
+              <a:t>f = 5</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -731,7 +819,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>c = 1</a:t>
+              <a:t>c = 5</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -741,7 +829,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>d = 4</a:t>
+              <a:t>d = 1</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -856,7 +944,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>f = 3</a:t>
+              <a:t>f = 4</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -866,7 +954,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>c = 3</a:t>
+              <a:t>c = 1</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -876,7 +964,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>d = 10</a:t>
+              <a:t>d = 1</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -904,8 +992,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7332132" y="2326216"/>
-          <a:ext cx="1390650" cy="1001184"/>
+          <a:off x="7284507" y="2326216"/>
+          <a:ext cx="1141942" cy="1001184"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -991,7 +1079,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>f = 3</a:t>
+              <a:t>f = 1</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1001,7 +1089,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>c = 5</a:t>
+              <a:t>c = 3</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1011,7 +1099,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>d = 4</a:t>
+              <a:t>d = 80</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1039,8 +1127,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9146116" y="2838450"/>
-          <a:ext cx="1390650" cy="1001184"/>
+          <a:off x="8701616" y="2838450"/>
+          <a:ext cx="1242484" cy="1001184"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -1126,7 +1214,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>f = 4</a:t>
+              <a:t>f = 2</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1136,7 +1224,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>c = 4</a:t>
+              <a:t>c = 2</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1146,7 +1234,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>d = 1</a:t>
+              <a:t>d = 64</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1174,7 +1262,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10843682" y="3244850"/>
+          <a:off x="10251016" y="3244850"/>
           <a:ext cx="1390650" cy="1001184"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
@@ -1271,7 +1359,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>c = 3</a:t>
+              <a:t>c = 1</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1281,7 +1369,7 @@
                   <a:schemeClr val="dk1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>d = -1</a:t>
+              <a:t>d = 1</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1950,8 +2038,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1883569" y="1976438"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="1897743" y="1995714"/>
+          <a:ext cx="947964" cy="423636"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2072,8 +2160,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1788319" y="2995614"/>
-          <a:ext cx="1095375" cy="723900"/>
+          <a:off x="1802493" y="3026230"/>
+          <a:ext cx="1090839" cy="732971"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2197,8 +2285,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3417094" y="1976438"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="3424464" y="1995714"/>
+          <a:ext cx="950232" cy="423636"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2319,8 +2407,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4817269" y="1985963"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="4822371" y="2005239"/>
+          <a:ext cx="947965" cy="423636"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2441,8 +2529,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11744325" y="2759869"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="11729017" y="2788217"/>
+          <a:ext cx="947964" cy="423635"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2821,8 +2909,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3264694" y="3043239"/>
-          <a:ext cx="1095375" cy="723900"/>
+          <a:off x="3274332" y="3073855"/>
+          <a:ext cx="1090839" cy="732971"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -2946,8 +3034,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4769644" y="3062289"/>
-          <a:ext cx="1302543" cy="723900"/>
+          <a:off x="4774746" y="3092905"/>
+          <a:ext cx="1298008" cy="732971"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -3071,8 +3159,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6276976" y="3078958"/>
-          <a:ext cx="1095375" cy="723900"/>
+          <a:off x="6277543" y="3109574"/>
+          <a:ext cx="1090839" cy="732971"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -3296,8 +3384,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4779169" y="4157663"/>
-          <a:ext cx="1095375" cy="723900"/>
+          <a:off x="4784271" y="4201886"/>
+          <a:ext cx="1090840" cy="732971"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -3804,8 +3892,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5545932" y="6415086"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="5548767" y="6486523"/>
+          <a:ext cx="947964" cy="423636"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -3979,8 +4067,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3960020" y="6412707"/>
-          <a:ext cx="952500" cy="419100"/>
+          <a:off x="3967390" y="6484144"/>
+          <a:ext cx="950232" cy="423636"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -4270,8 +4358,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1190626" y="6465094"/>
-          <a:ext cx="952500" cy="476252"/>
+          <a:off x="1204800" y="6536531"/>
+          <a:ext cx="950232" cy="483056"/>
           <a:chOff x="1924050" y="419100"/>
           <a:chExt cx="1085850" cy="666750"/>
         </a:xfrm>
@@ -4936,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
@@ -5021,10 +5109,10 @@
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
@@ -5195,21 +5283,21 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="G15" s="18"/>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="46" t="s">
-        <v>35</v>
+      <c r="I16" s="39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
@@ -5227,8 +5315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:H14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5299,10 +5387,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -5333,9 +5421,9 @@
       <c r="H5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="46"/>
+      <c r="J5" s="39"/>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -5367,7 +5455,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -5393,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -5419,12 +5507,12 @@
         <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" s="50">
+      <c r="P9" s="43">
         <v>2</v>
       </c>
     </row>
@@ -5455,7 +5543,7 @@
       </c>
       <c r="L10" s="4"/>
       <c r="M10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -5471,13 +5559,13 @@
       <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="40">
         <v>0</v>
       </c>
       <c r="G11" s="23">
         <v>1</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="41">
         <v>2</v>
       </c>
       <c r="I11" s="25">
@@ -5506,10 +5594,10 @@
       <c r="G12" s="22">
         <v>4</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="42">
         <v>1</v>
       </c>
-      <c r="I12" s="51">
+      <c r="I12" s="44">
         <v>3</v>
       </c>
       <c r="K12" s="13">
@@ -5517,7 +5605,7 @@
       </c>
       <c r="L12" s="4"/>
       <c r="O12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="P12">
         <v>15</v>
@@ -5525,7 +5613,7 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -5572,7 +5660,7 @@
         <v>5</v>
       </c>
       <c r="M14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -5581,7 +5669,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -5607,7 +5695,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -5630,7 +5718,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -5652,7 +5740,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -5663,10 +5751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N36"/>
+  <dimension ref="B2:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R4" sqref="R3:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5675,164 +5763,274 @@
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="27"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34">
         <v>1</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="34">
         <v>2</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="34">
         <v>3</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="34">
         <v>4</v>
       </c>
-      <c r="H2" s="41">
+      <c r="H2" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34">
+        <v>1</v>
+      </c>
+      <c r="L2" s="34">
+        <v>2</v>
+      </c>
+      <c r="M2" s="34">
+        <v>3</v>
+      </c>
+      <c r="N2" s="34">
+        <v>4</v>
+      </c>
+      <c r="O2" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="35">
         <v>1</v>
       </c>
-      <c r="D3" s="43">
-        <v>0</v>
-      </c>
-      <c r="E3" s="44">
-        <v>0</v>
-      </c>
-      <c r="F3" s="44">
-        <v>0</v>
-      </c>
-      <c r="G3" s="44">
-        <v>0</v>
-      </c>
-      <c r="H3" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="D3" s="36">
+        <v>1</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0</v>
+      </c>
+      <c r="F3" s="37">
+        <v>80</v>
+      </c>
+      <c r="G3" s="37">
+        <v>0</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0</v>
+      </c>
+      <c r="J3" s="35">
+        <v>1</v>
+      </c>
+      <c r="K3" s="36">
+        <v>99</v>
+      </c>
+      <c r="L3" s="37">
+        <v>0</v>
+      </c>
+      <c r="M3" s="37">
+        <v>0</v>
+      </c>
+      <c r="N3" s="37">
+        <v>0</v>
+      </c>
+      <c r="O3" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="27"/>
-      <c r="C4" s="42">
+      <c r="C4" s="35">
         <v>2</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="36">
+        <v>0</v>
+      </c>
+      <c r="E4" s="37">
+        <v>64</v>
+      </c>
+      <c r="F4" s="37">
+        <v>0</v>
+      </c>
+      <c r="G4" s="37">
+        <v>0</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0</v>
+      </c>
+      <c r="J4" s="35">
+        <v>2</v>
+      </c>
+      <c r="K4" s="36">
+        <v>0</v>
+      </c>
+      <c r="L4" s="37">
+        <v>99</v>
+      </c>
+      <c r="M4" s="37">
+        <v>0</v>
+      </c>
+      <c r="N4" s="37">
+        <v>0</v>
+      </c>
+      <c r="O4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="27"/>
+      <c r="C5" s="35">
+        <v>3</v>
+      </c>
+      <c r="D5" s="36">
+        <v>0</v>
+      </c>
+      <c r="E5" s="37">
+        <v>0</v>
+      </c>
+      <c r="F5" s="37">
+        <v>0</v>
+      </c>
+      <c r="G5" s="37">
+        <v>0</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0</v>
+      </c>
+      <c r="J5" s="35">
+        <v>3</v>
+      </c>
+      <c r="K5" s="36">
+        <v>0</v>
+      </c>
+      <c r="L5" s="37">
+        <v>0</v>
+      </c>
+      <c r="M5" s="37">
+        <v>0</v>
+      </c>
+      <c r="N5" s="37">
+        <v>0</v>
+      </c>
+      <c r="O5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="27"/>
+      <c r="C6" s="35">
         <v>4</v>
       </c>
-      <c r="E4" s="44">
-        <v>0</v>
-      </c>
-      <c r="F4" s="44">
-        <v>0</v>
-      </c>
-      <c r="G4" s="44">
-        <v>0</v>
-      </c>
-      <c r="H4" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="42">
-        <v>3</v>
-      </c>
-      <c r="D5" s="43">
-        <v>0</v>
-      </c>
-      <c r="E5" s="44">
-        <v>0</v>
-      </c>
-      <c r="F5" s="44">
-        <v>2</v>
-      </c>
-      <c r="G5" s="44">
-        <v>0</v>
-      </c>
-      <c r="H5" s="45">
+      <c r="D6" s="36">
+        <v>0</v>
+      </c>
+      <c r="E6" s="37">
+        <v>0</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0</v>
+      </c>
+      <c r="G6" s="37">
+        <v>1</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0</v>
+      </c>
+      <c r="J6" s="35">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="27"/>
-      <c r="C6" s="42">
-        <v>4</v>
-      </c>
-      <c r="D6" s="43">
-        <v>0</v>
-      </c>
-      <c r="E6" s="44">
-        <v>0</v>
-      </c>
-      <c r="F6" s="44">
-        <v>0</v>
-      </c>
-      <c r="G6" s="44">
+      <c r="K6" s="36">
+        <v>0</v>
+      </c>
+      <c r="L6" s="37">
+        <v>0</v>
+      </c>
+      <c r="M6" s="37">
+        <v>0</v>
+      </c>
+      <c r="N6" s="37">
+        <v>0</v>
+      </c>
+      <c r="O6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="27"/>
+      <c r="C7" s="35">
+        <v>5</v>
+      </c>
+      <c r="D7" s="36">
+        <v>0</v>
+      </c>
+      <c r="E7" s="37">
+        <v>0</v>
+      </c>
+      <c r="F7" s="37">
+        <v>0</v>
+      </c>
+      <c r="G7" s="37">
+        <v>0</v>
+      </c>
+      <c r="H7" s="38">
         <v>1</v>
       </c>
-      <c r="H6" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="27"/>
-      <c r="C7" s="42">
+      <c r="J7" s="35">
         <v>5</v>
       </c>
-      <c r="D7" s="43">
-        <v>0</v>
-      </c>
-      <c r="E7" s="44">
-        <v>0</v>
-      </c>
-      <c r="F7" s="44">
-        <v>0</v>
-      </c>
-      <c r="G7" s="44">
-        <v>0</v>
-      </c>
-      <c r="H7" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K7" s="36">
+        <v>0</v>
+      </c>
+      <c r="L7" s="37">
+        <v>0</v>
+      </c>
+      <c r="M7" s="37">
+        <v>0</v>
+      </c>
+      <c r="N7" s="37">
+        <v>0</v>
+      </c>
+      <c r="O7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
@@ -5840,152 +6038,638 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G20" s="5"/>
-      <c r="J20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="E26" s="34"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" ht="21" x14ac:dyDescent="0.3">
+      <c r="B26" s="27"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34">
+        <v>1</v>
+      </c>
+      <c r="E26" s="34">
+        <v>2</v>
+      </c>
       <c r="F26" s="34">
+        <v>3</v>
+      </c>
+      <c r="G26" s="34">
+        <v>4</v>
+      </c>
+      <c r="H26" s="34">
+        <v>5</v>
+      </c>
+      <c r="J26" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="P26" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q26" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="R26" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="T26" s="47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="35">
         <v>1</v>
       </c>
-      <c r="G26" s="34">
+      <c r="D27" s="36">
+        <v>1</v>
+      </c>
+      <c r="E27" s="37">
+        <v>0</v>
+      </c>
+      <c r="F27" s="37">
+        <v>80</v>
+      </c>
+      <c r="G27" s="37">
+        <v>1</v>
+      </c>
+      <c r="H27" s="38">
+        <v>0</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="48">
+        <v>1</v>
+      </c>
+      <c r="L27" s="48">
+        <v>1</v>
+      </c>
+      <c r="M27" s="48">
+        <v>1</v>
+      </c>
+      <c r="N27" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="P27" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q27" s="51">
+        <v>1</v>
+      </c>
+      <c r="R27" s="51">
         <v>2</v>
       </c>
-      <c r="H26" s="34">
+      <c r="S27" s="51">
+        <v>0</v>
+      </c>
+      <c r="T27" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="27"/>
+      <c r="C28" s="35">
+        <v>2</v>
+      </c>
+      <c r="D28" s="36">
+        <v>0</v>
+      </c>
+      <c r="E28" s="37">
+        <v>64</v>
+      </c>
+      <c r="F28" s="37">
+        <v>0</v>
+      </c>
+      <c r="G28" s="37">
+        <v>1</v>
+      </c>
+      <c r="H28" s="38">
+        <v>0</v>
+      </c>
+      <c r="J28" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28" s="46">
+        <v>1</v>
+      </c>
+      <c r="L28" s="46">
         <v>3</v>
       </c>
-      <c r="I26" s="34">
+      <c r="M28" s="45">
+        <v>80</v>
+      </c>
+      <c r="N28" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="P28" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q28" s="46">
+        <v>1</v>
+      </c>
+      <c r="R28" s="46">
+        <v>3</v>
+      </c>
+      <c r="S28" s="45">
+        <v>80</v>
+      </c>
+      <c r="T28" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="27"/>
+      <c r="C29" s="35">
+        <v>3</v>
+      </c>
+      <c r="D29" s="36">
+        <v>0</v>
+      </c>
+      <c r="E29" s="37">
+        <v>0</v>
+      </c>
+      <c r="F29" s="37">
+        <v>1</v>
+      </c>
+      <c r="G29" s="37">
+        <v>0</v>
+      </c>
+      <c r="H29" s="38">
+        <v>1</v>
+      </c>
+      <c r="J29" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29" s="48">
+        <v>1</v>
+      </c>
+      <c r="L29" s="48">
         <v>4</v>
       </c>
-      <c r="J26" s="34">
+      <c r="M29" s="48">
+        <v>1</v>
+      </c>
+      <c r="N29" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="P29" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q29" s="51">
+        <v>1</v>
+      </c>
+      <c r="R29" s="51">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E27" s="35">
+      <c r="S29" s="51">
+        <v>0</v>
+      </c>
+      <c r="T29" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="B30" s="27"/>
+      <c r="C30" s="35">
+        <v>4</v>
+      </c>
+      <c r="D30" s="36">
         <v>1</v>
       </c>
-      <c r="F27" s="36">
+      <c r="E30" s="37">
+        <v>1</v>
+      </c>
+      <c r="F30" s="37">
+        <v>0</v>
+      </c>
+      <c r="G30" s="37">
+        <v>1</v>
+      </c>
+      <c r="H30" s="38">
+        <v>0</v>
+      </c>
+      <c r="J30" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="46">
+        <v>2</v>
+      </c>
+      <c r="L30" s="46">
+        <v>2</v>
+      </c>
+      <c r="M30" s="46">
+        <v>64</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="O30" s="39"/>
+      <c r="P30" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q30" s="51">
+        <v>2</v>
+      </c>
+      <c r="R30" s="51">
+        <v>1</v>
+      </c>
+      <c r="S30" s="51">
+        <v>0</v>
+      </c>
+      <c r="T30" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="B31" s="27"/>
+      <c r="C31" s="35">
+        <v>5</v>
+      </c>
+      <c r="D31" s="36">
+        <v>0</v>
+      </c>
+      <c r="E31" s="37">
+        <v>0</v>
+      </c>
+      <c r="F31" s="37">
+        <v>0</v>
+      </c>
+      <c r="G31" s="37">
+        <v>0</v>
+      </c>
+      <c r="H31" s="38">
+        <v>1</v>
+      </c>
+      <c r="J31" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K31" s="48">
+        <v>2</v>
+      </c>
+      <c r="L31" s="48">
+        <v>4</v>
+      </c>
+      <c r="M31" s="48">
+        <v>1</v>
+      </c>
+      <c r="N31" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="P31" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" s="46">
+        <v>2</v>
+      </c>
+      <c r="R31" s="46">
+        <v>2</v>
+      </c>
+      <c r="S31" s="46">
+        <v>64</v>
+      </c>
+      <c r="T31" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J32" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="48">
+        <v>3</v>
+      </c>
+      <c r="L32" s="48">
+        <v>3</v>
+      </c>
+      <c r="M32" s="48">
+        <v>1</v>
+      </c>
+      <c r="N32" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="P32" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q32" s="50">
+        <v>2</v>
+      </c>
+      <c r="R32" s="50">
+        <v>3</v>
+      </c>
+      <c r="S32" s="50">
+        <v>0</v>
+      </c>
+      <c r="T32" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+      <c r="J33" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="48">
+        <v>3</v>
+      </c>
+      <c r="L33" s="48">
+        <v>5</v>
+      </c>
+      <c r="M33" s="48">
+        <v>1</v>
+      </c>
+      <c r="N33" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="P33" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q33" s="50">
+        <v>2</v>
+      </c>
+      <c r="R33" s="50">
+        <v>5</v>
+      </c>
+      <c r="S33" s="50">
+        <v>0</v>
+      </c>
+      <c r="T33" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="48">
+        <v>4</v>
+      </c>
+      <c r="L34" s="48">
+        <v>1</v>
+      </c>
+      <c r="M34" s="48">
+        <v>1</v>
+      </c>
+      <c r="N34" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="P34" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q34" s="50">
+        <v>3</v>
+      </c>
+      <c r="R34" s="50">
+        <v>1</v>
+      </c>
+      <c r="S34" s="50">
+        <v>0</v>
+      </c>
+      <c r="T34" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J35" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="48">
+        <v>4</v>
+      </c>
+      <c r="L35" s="48">
+        <v>2</v>
+      </c>
+      <c r="M35" s="48">
+        <v>1</v>
+      </c>
+      <c r="N35" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="P35" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q35" s="50">
+        <v>3</v>
+      </c>
+      <c r="R35" s="50">
+        <v>2</v>
+      </c>
+      <c r="S35" s="50">
+        <v>0</v>
+      </c>
+      <c r="T35" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J36" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="48">
+        <v>4</v>
+      </c>
+      <c r="L36" s="48">
+        <v>4</v>
+      </c>
+      <c r="M36" s="48">
+        <v>1</v>
+      </c>
+      <c r="N36" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="P36" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q36" s="50">
+        <v>3</v>
+      </c>
+      <c r="R36" s="50">
+        <v>4</v>
+      </c>
+      <c r="S36" s="50">
+        <v>0</v>
+      </c>
+      <c r="T36" s="45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J37" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="48">
+        <v>5</v>
+      </c>
+      <c r="L37" s="48">
+        <v>5</v>
+      </c>
+      <c r="M37" s="48">
+        <v>1</v>
+      </c>
+      <c r="N37" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="P37" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q37" s="50">
+        <v>4</v>
+      </c>
+      <c r="R37" s="50">
+        <v>3</v>
+      </c>
+      <c r="S37" s="50">
+        <v>0</v>
+      </c>
+      <c r="T37" s="45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J38" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="P38" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q38" s="50">
+        <v>4</v>
+      </c>
+      <c r="R38" s="50">
+        <v>5</v>
+      </c>
+      <c r="S38" s="50">
+        <v>0</v>
+      </c>
+      <c r="T38" s="45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J39" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="K39" t="s">
+        <v>82</v>
+      </c>
+      <c r="L39" t="s">
+        <v>83</v>
+      </c>
+      <c r="P39" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q39" s="50">
+        <v>5</v>
+      </c>
+      <c r="R39" s="50">
+        <v>1</v>
+      </c>
+      <c r="S39" s="50">
+        <v>0</v>
+      </c>
+      <c r="T39" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40" s="48">
+        <v>9</v>
+      </c>
+      <c r="L40" s="48">
         <v>14</v>
       </c>
-      <c r="G27" s="37">
-        <v>0</v>
-      </c>
-      <c r="H27" s="39">
-        <v>1</v>
-      </c>
-      <c r="I27" s="37">
-        <v>1</v>
-      </c>
-      <c r="J27" s="38">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>30</v>
-      </c>
-      <c r="N27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E28" s="35">
+      <c r="M40">
+        <f>SUM(J40:L40)</f>
+        <v>25</v>
+      </c>
+      <c r="P40" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" s="50">
+        <v>5</v>
+      </c>
+      <c r="R40" s="50">
         <v>2</v>
       </c>
-      <c r="F28" s="36">
-        <v>0</v>
-      </c>
-      <c r="G28" s="40">
-        <v>11</v>
-      </c>
-      <c r="H28" s="39">
-        <v>0</v>
-      </c>
-      <c r="I28" s="37">
-        <v>14</v>
-      </c>
-      <c r="J28" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E29" s="35">
+      <c r="S40" s="50">
+        <v>0</v>
+      </c>
+      <c r="T40" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="P41" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q41" s="50">
+        <v>5</v>
+      </c>
+      <c r="R41" s="50">
         <v>3</v>
       </c>
-      <c r="F29" s="36">
-        <v>0</v>
-      </c>
-      <c r="G29" s="37">
-        <v>0</v>
-      </c>
-      <c r="H29" s="39">
-        <v>0</v>
-      </c>
-      <c r="I29" s="37">
-        <v>0</v>
-      </c>
-      <c r="J29" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E30" s="35">
+      <c r="S41" s="50">
+        <v>0</v>
+      </c>
+      <c r="T41" s="45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="P42" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q42" s="50">
+        <v>5</v>
+      </c>
+      <c r="R42" s="50">
         <v>4</v>
       </c>
-      <c r="F30" s="36">
-        <v>0</v>
-      </c>
-      <c r="G30" s="37">
-        <v>0</v>
-      </c>
-      <c r="H30" s="39">
-        <v>0</v>
-      </c>
-      <c r="I30" s="37">
-        <v>0</v>
-      </c>
-      <c r="J30" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E31" s="35">
-        <v>5</v>
-      </c>
-      <c r="F31" s="36">
-        <v>0</v>
-      </c>
-      <c r="G31" s="37">
-        <v>0</v>
-      </c>
-      <c r="H31" s="39">
-        <v>0</v>
-      </c>
-      <c r="I31" s="37">
-        <v>0</v>
-      </c>
-      <c r="J31" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="G35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" t="s">
-        <v>28</v>
+      <c r="S42" s="50">
+        <v>0</v>
+      </c>
+      <c r="T42" s="45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="P43" s="47" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5999,7 +6683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -6138,27 +6822,27 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -6179,18 +6863,18 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>